<commit_message>
from my office machine
</commit_message>
<xml_diff>
--- a/SIMPLETEST/INTERVIEW QUESTIONS/JAVASCRIPT.xlsx
+++ b/SIMPLETEST/INTERVIEW QUESTIONS/JAVASCRIPT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,15 +15,143 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Primitives are passed by value, i.e. a copy of the primitive itself is passed. Whereas for objects, the copy of the reference is passed, not the object itself.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>What is the difference between a function call and function reference?</t>
+  </si>
+  <si>
+    <t>Function Declarations vs. Function Expressions</t>
+  </si>
+  <si>
+    <t>Difference between jQuery parent() and closest() functions?</t>
+  </si>
+  <si>
+    <t>What is a prototype?</t>
+  </si>
+  <si>
+    <t>A prototype is an object from which other objects inherit properties</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">undefined , null , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>boolean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and number</t>
+    </r>
+  </si>
+  <si>
+    <t>5 primitive types</t>
+  </si>
+  <si>
+    <t>object vs. primitive</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,14 +174,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -132,6 +266,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -166,6 +301,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -341,36 +477,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.140625" customWidth="1"/>
+    <col min="2" max="2" width="115.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>